<commit_message>
Cleaning up Updates a little
</commit_message>
<xml_diff>
--- a/plans/Plans.xlsx
+++ b/plans/Plans.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="173">
   <si>
     <t>Fall 2016</t>
   </si>
@@ -606,9 +606,6 @@
   </si>
   <si>
     <t>Or replace data mining with NLP?</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
 </sst>
 </file>
@@ -722,13 +719,13 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -792,10 +789,10 @@
   <tableColumns count="6">
     <tableColumn id="1" name="Department" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Number"/>
-    <tableColumn id="6" name="Code" dataDxfId="1">
+    <tableColumn id="6" name="Code" dataDxfId="9">
       <calculatedColumnFormula>Spring_2017[[#This Row],[Department]] &amp; " " &amp; Spring_2017[[#This Row],[Number]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Description" dataDxfId="0">
+    <tableColumn id="3" name="Description" dataDxfId="8">
       <calculatedColumnFormula>IF(AND(ISBLANK(Spring_2017[[#This Row],[Department]]), ISBLANK(Spring_2017[[#This Row],[Number]])), "Elective", VLOOKUP(Spring_2017[[#This Row],[Department]] &amp; " " &amp; Spring_2017[[#This Row],[Number]], Courses[], 4, FALSE))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="Reg Crd" totalsRowFunction="sum"/>
@@ -811,10 +808,10 @@
   <tableColumns count="6">
     <tableColumn id="1" name="Department" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Number"/>
-    <tableColumn id="6" name="Code" dataDxfId="9">
+    <tableColumn id="6" name="Code" dataDxfId="7">
       <calculatedColumnFormula>Fall_2017[[#This Row],[Department]] &amp; " " &amp; Fall_2017[[#This Row],[Number]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Description" dataDxfId="8">
+    <tableColumn id="3" name="Description" dataDxfId="6">
       <calculatedColumnFormula>IF(AND(ISBLANK(Fall_2017[[#This Row],[Department]]), ISBLANK(Fall_2017[[#This Row],[Number]])), "Elective", VLOOKUP(Fall_2017[[#This Row],[Department]] &amp; " " &amp; Fall_2017[[#This Row],[Number]], Courses[], 4, FALSE))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="Reg Crd" totalsRowFunction="sum"/>
@@ -830,7 +827,7 @@
   <tableColumns count="6">
     <tableColumn id="1" name="Department" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Number"/>
-    <tableColumn id="6" name="Code" dataDxfId="7">
+    <tableColumn id="6" name="Code" dataDxfId="5">
       <calculatedColumnFormula>Summer_2017[[#This Row],[Department]] &amp; " " &amp; Summer_2017[[#This Row],[Number]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="Description"/>
@@ -847,10 +844,10 @@
   <tableColumns count="6">
     <tableColumn id="1" name="Department" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Number"/>
-    <tableColumn id="6" name="Code" dataDxfId="6">
+    <tableColumn id="6" name="Code" dataDxfId="4">
       <calculatedColumnFormula>Spring_2018[[#This Row],[Department]] &amp; " " &amp; Spring_2018[[#This Row],[Number]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Description" dataDxfId="5">
+    <tableColumn id="3" name="Description" dataDxfId="3">
       <calculatedColumnFormula>IF(AND(ISBLANK(Spring_2018[[#This Row],[Department]]), ISBLANK(Spring_2018[[#This Row],[Number]])), "Elective", VLOOKUP(Spring_2018[[#This Row],[Department]] &amp; " " &amp; Spring_2018[[#This Row],[Number]], Courses[], 4, FALSE))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="Reg Crd" totalsRowFunction="sum"/>
@@ -879,11 +876,11 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="12">
-    <tableColumn id="1" name="Code" dataDxfId="4" dataCellStyle="Normal">
+    <tableColumn id="1" name="Code" dataDxfId="2" dataCellStyle="Normal">
       <calculatedColumnFormula>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="12" name="Dpmt" dataCellStyle="Normal"/>
-    <tableColumn id="11" name="Num" dataDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="11" name="Num" dataDxfId="1" dataCellStyle="Normal"/>
     <tableColumn id="2" name="Description" dataCellStyle="Normal"/>
     <tableColumn id="3" name="Semester" dataCellStyle="Normal"/>
     <tableColumn id="4" name="Comments" dataCellStyle="Normal"/>
@@ -898,7 +895,7 @@
     <tableColumn id="9" name="Fall 2017" dataCellStyle="Normal">
       <calculatedColumnFormula array="1">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Spring 2018" dataDxfId="2" dataCellStyle="Normal">
+    <tableColumn id="10" name="Spring 2018" dataDxfId="0" dataCellStyle="Normal">
       <calculatedColumnFormula array="1">IF( SUM((Courses[[#This Row],[Code]] = Spring_2018[Code]) * 1), TRUE(), "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1196,7 +1193,7 @@
   <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1570,9 +1567,6 @@
       </c>
       <c r="F14">
         <v>3</v>
-      </c>
-      <c r="H14" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Lots of updates to my interests and Updates
</commit_message>
<xml_diff>
--- a/plans/Plans.xlsx
+++ b/plans/Plans.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="173">
   <si>
     <t>Fall 2016</t>
   </si>
@@ -861,20 +861,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Courses" displayName="Courses" ref="A1:L58" totalsRowShown="0" dataCellStyle="Normal">
   <autoFilter ref="A1:L58">
     <filterColumn colId="7">
-      <filters>
+      <filters blank="1">
+        <filter val="DY"/>
         <filter val="MY"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="8">
-      <filters blank="1"/>
-    </filterColumn>
-    <filterColumn colId="9">
-      <filters blank="1"/>
-    </filterColumn>
-    <filterColumn colId="10">
-      <filters blank="1"/>
-    </filterColumn>
   </autoFilter>
+  <sortState ref="A2:L58">
+    <sortCondition ref="H1:H58"/>
+  </sortState>
   <tableColumns count="12">
     <tableColumn id="1" name="Code" dataDxfId="2" dataCellStyle="Normal">
       <calculatedColumnFormula>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</calculatedColumnFormula>
@@ -1193,7 +1188,7 @@
   <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1552,15 +1547,15 @@
         <v>5</v>
       </c>
       <c r="B14">
-        <v>6012</v>
+        <v>6016</v>
       </c>
       <c r="C14" t="str">
         <f>Spring_2017[[#This Row],[Department]] &amp; " " &amp; Spring_2017[[#This Row],[Number]]</f>
-        <v>SYS 6012</v>
+        <v>SYS 6016</v>
       </c>
       <c r="D14" t="str">
         <f>IF(AND(ISBLANK(Spring_2017[[#This Row],[Department]]), ISBLANK(Spring_2017[[#This Row],[Number]])), "Elective", VLOOKUP(Spring_2017[[#This Row],[Department]] &amp; " " &amp; Spring_2017[[#This Row],[Number]], Courses[], 4, FALSE))</f>
-        <v>Dynamic Systems</v>
+        <v>Machine Learning</v>
       </c>
       <c r="E14">
         <v>3</v>
@@ -1760,13 +1755,19 @@
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28">
+        <v>6012</v>
+      </c>
       <c r="C28" t="str">
         <f>Fall_2017[[#This Row],[Department]] &amp; " " &amp; Fall_2017[[#This Row],[Number]]</f>
-        <v xml:space="preserve"> </v>
+        <v>SYS 6012</v>
       </c>
       <c r="D28" t="str">
         <f>IF(AND(ISBLANK(Fall_2017[[#This Row],[Department]]), ISBLANK(Fall_2017[[#This Row],[Number]])), "Elective", VLOOKUP(Fall_2017[[#This Row],[Department]] &amp; " " &amp; Fall_2017[[#This Row],[Number]], Courses[], 4, FALSE))</f>
-        <v>Elective</v>
+        <v>Dynamic Systems</v>
       </c>
       <c r="E28">
         <v>3</v>
@@ -1859,13 +1860,19 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35">
+        <v>6023</v>
+      </c>
       <c r="C35" t="str">
         <f>Spring_2018[[#This Row],[Department]] &amp; " " &amp; Spring_2018[[#This Row],[Number]]</f>
-        <v xml:space="preserve"> </v>
+        <v>SYS 6023</v>
       </c>
       <c r="D35" t="str">
         <f>IF(AND(ISBLANK(Spring_2018[[#This Row],[Department]]), ISBLANK(Spring_2018[[#This Row],[Number]])), "Elective", VLOOKUP(Spring_2018[[#This Row],[Department]] &amp; " " &amp; Spring_2018[[#This Row],[Number]], Courses[], 4, FALSE))</f>
-        <v>Elective</v>
+        <v>Cognitive Systems Engineering</v>
       </c>
       <c r="E35">
         <v>3</v>
@@ -1971,7 +1978,7 @@
   <dimension ref="A1:N58"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2028,34 +2035,36 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 6001</v>
+        <v>SYS 6016</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="9">
-        <v>6001</v>
+        <v>6016</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="E2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G2" t="b">
-        <f>TRUE()</f>
+        <v>97</v>
+      </c>
+      <c r="G2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" t="s">
+        <v>138</v>
+      </c>
+      <c r="I2" t="str">
+        <f t="array" ref="I2">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="J2" t="b">
+        <f t="array" ref="J2">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
         <v>1</v>
-      </c>
-      <c r="I2" t="b">
-        <f t="array" ref="I2">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
-        <v>1</v>
-      </c>
-      <c r="J2" t="str">
-        <f t="array" ref="J2">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
-        <v/>
       </c>
       <c r="K2" t="str">
         <f t="array" ref="K2">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
@@ -2109,76 +2118,83 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 6003</v>
+        <v>SYS 6018</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="9">
-        <v>6003</v>
+        <v>6018</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E4" t="s">
-        <v>95</v>
-      </c>
-      <c r="G4" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
+        <v>101</v>
+      </c>
+      <c r="F4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4" t="s">
+        <v>155</v>
+      </c>
+      <c r="H4" t="s">
+        <v>138</v>
       </c>
       <c r="I4" t="str">
         <f t="array" ref="I4">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
         <v/>
       </c>
-      <c r="J4" t="str">
+      <c r="J4" t="b">
         <f t="array" ref="J4">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="K4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" t="str">
         <f t="array" ref="K4">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="L4" t="str">
         <f t="array" ref="L4">IF( SUM((Courses[[#This Row],[Code]] = Spring_2018[Code]) * 1), TRUE(), "")</f>
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 6005</v>
+        <v>SYS 6012</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="9">
-        <v>6005</v>
+        <v>6012</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
         <v>95</v>
       </c>
-      <c r="G5" t="b">
-        <f>TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I5" t="b">
+      <c r="G5" t="s">
+        <v>155</v>
+      </c>
+      <c r="H5" t="s">
+        <v>137</v>
+      </c>
+      <c r="I5" t="str">
         <f t="array" ref="I5">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="J5" t="str">
         <f t="array" ref="J5">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
         <v/>
       </c>
-      <c r="K5" t="str">
+      <c r="K5" t="b">
         <f t="array" ref="K5">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="L5" t="str">
         <f t="array" ref="L5">IF( SUM((Courses[[#This Row],[Code]] = Spring_2018[Code]) * 1), TRUE(), "")</f>
@@ -2225,22 +2241,22 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 6012</v>
+        <v>SYS 6023</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="9">
-        <v>6012</v>
+        <v>6023</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="E7" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="G7" t="s">
         <v>155</v>
@@ -2252,35 +2268,41 @@
         <f t="array" ref="I7">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
         <v/>
       </c>
-      <c r="J7" t="b">
+      <c r="J7" t="str">
         <f t="array" ref="J7">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="K7" t="str">
         <f t="array" ref="K7">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
         <v/>
       </c>
-      <c r="L7" t="str">
+      <c r="L7" t="b">
         <f t="array" ref="L7">IF( SUM((Courses[[#This Row],[Code]] = Spring_2018[Code]) * 1), TRUE(), "")</f>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 6013</v>
+        <v>SYS 6034</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="9">
-        <v>6013</v>
+        <v>6034</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>70</v>
+      </c>
+      <c r="E8" t="s">
+        <v>95</v>
       </c>
       <c r="G8" t="s">
         <v>155</v>
+      </c>
+      <c r="H8" t="s">
+        <v>137</v>
       </c>
       <c r="I8" t="str">
         <f t="array" ref="I8">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
@@ -2305,30 +2327,33 @@
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 6014</v>
+        <v>SYS 6035</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="9">
-        <v>6014</v>
+        <v>6035</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="E9" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="G9" t="s">
         <v>155</v>
+      </c>
+      <c r="H9" t="s">
+        <v>137</v>
       </c>
       <c r="I9" t="str">
         <f t="array" ref="I9">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
         <v/>
       </c>
-      <c r="J9" t="str">
+      <c r="J9" t="b">
         <f t="array" ref="J9">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="K9" t="str">
         <f t="array" ref="K9">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
@@ -2342,28 +2367,31 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 6016</v>
+        <v>SYS 6044</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="9">
-        <v>6016</v>
+        <v>6044</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="E10" t="s">
-        <v>97</v>
+        <v>117</v>
+      </c>
+      <c r="F10" t="s">
+        <v>130</v>
       </c>
       <c r="G10" t="s">
         <v>155</v>
       </c>
       <c r="H10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I10" t="str">
         <f t="array" ref="I10">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
@@ -2382,39 +2410,36 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 6018</v>
+        <v>SYS 7001</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="9">
-        <v>6018</v>
+        <v>7001</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="E11" t="s">
-        <v>101</v>
-      </c>
-      <c r="F11" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="G11" t="s">
         <v>155</v>
       </c>
       <c r="H11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I11" t="str">
         <f t="array" ref="I11">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
         <v/>
       </c>
-      <c r="J11" t="b">
+      <c r="J11" t="str">
         <f t="array" ref="J11">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="K11" t="str">
         <f t="array" ref="K11">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
@@ -2471,19 +2496,19 @@
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 6023</v>
+        <v>SOC 5120</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>5</v>
+        <v>163</v>
       </c>
       <c r="C13" s="9">
-        <v>6023</v>
+        <v>5120</v>
       </c>
       <c r="D13" t="s">
-        <v>68</v>
+        <v>152</v>
       </c>
       <c r="E13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G13" t="s">
         <v>155</v>
@@ -2514,22 +2539,25 @@
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 6026</v>
+        <v>PSYC 7700</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>5</v>
+        <v>164</v>
       </c>
       <c r="C14" s="9">
-        <v>6026</v>
+        <v>7700</v>
       </c>
       <c r="D14" t="s">
-        <v>69</v>
+        <v>160</v>
       </c>
       <c r="E14" t="s">
-        <v>102</v>
+        <v>161</v>
       </c>
       <c r="G14" t="s">
         <v>155</v>
+      </c>
+      <c r="H14" t="s">
+        <v>137</v>
       </c>
       <c r="I14" t="str">
         <f t="array" ref="I14">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
@@ -2549,61 +2577,65 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="str">
-        <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 6034</v>
+      <c r="A15" s="8" t="str">
+        <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
+        <v>PSYC 8730</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>5</v>
+        <v>164</v>
       </c>
       <c r="C15" s="9">
-        <v>6034</v>
-      </c>
-      <c r="D15" t="s">
-        <v>70</v>
-      </c>
-      <c r="E15" t="s">
-        <v>95</v>
-      </c>
+        <v>8730</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="F15" s="7"/>
       <c r="G15" t="s">
         <v>155</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="I15" t="str">
+      <c r="I15" s="7" t="str">
         <f t="array" ref="I15">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
         <v/>
       </c>
-      <c r="J15" t="str">
+      <c r="J15" s="7" t="str">
         <f t="array" ref="J15">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
         <v/>
       </c>
-      <c r="K15" t="str">
+      <c r="K15" s="7" t="str">
         <f t="array" ref="K15">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
         <v/>
       </c>
-      <c r="L15" t="str">
+      <c r="L15" s="8" t="str">
         <f t="array" ref="L15">IF( SUM((Courses[[#This Row],[Code]] = Spring_2018[Code]) * 1), TRUE(), "")</f>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 6035</v>
+        <v>PLAN 5630</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>5</v>
+        <v>139</v>
       </c>
       <c r="C16" s="9">
-        <v>6035</v>
+        <v>5630</v>
       </c>
       <c r="D16" t="s">
-        <v>71</v>
+        <v>150</v>
       </c>
       <c r="E16" t="s">
-        <v>103</v>
+        <v>159</v>
+      </c>
+      <c r="F16" t="s">
+        <v>151</v>
       </c>
       <c r="G16" t="s">
         <v>155</v>
@@ -2615,9 +2647,9 @@
         <f t="array" ref="I16">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
         <v/>
       </c>
-      <c r="J16" t="b">
+      <c r="J16" t="str">
         <f t="array" ref="J16">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="K16" t="str">
         <f t="array" ref="K16">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
@@ -2631,19 +2663,25 @@
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 6042</v>
+        <v>PPOL 5025</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>5</v>
+        <v>153</v>
       </c>
       <c r="C17" s="9">
-        <v>6042</v>
+        <v>5025</v>
       </c>
       <c r="D17" t="s">
-        <v>72</v>
+        <v>154</v>
+      </c>
+      <c r="E17" t="s">
+        <v>158</v>
       </c>
       <c r="G17" t="s">
         <v>155</v>
+      </c>
+      <c r="H17" t="s">
+        <v>137</v>
       </c>
       <c r="I17" t="str">
         <f t="array" ref="I17">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
@@ -2665,23 +2703,27 @@
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 6043</v>
+        <v>SYS 6001</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="9">
-        <v>6043</v>
+        <v>6001</v>
       </c>
       <c r="D18" t="s">
-        <v>73</v>
-      </c>
-      <c r="G18" t="s">
-        <v>155</v>
-      </c>
-      <c r="I18" t="str">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>95</v>
+      </c>
+      <c r="G18" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I18" t="b">
         <f t="array" ref="I18">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="J18" t="str">
         <f t="array" ref="J18">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
@@ -2699,28 +2741,23 @@
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 6044</v>
+        <v>SYS 6003</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="9">
-        <v>6044</v>
+        <v>6003</v>
       </c>
       <c r="D19" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="E19" t="s">
-        <v>117</v>
-      </c>
-      <c r="F19" t="s">
-        <v>130</v>
-      </c>
-      <c r="G19" t="s">
-        <v>155</v>
-      </c>
-      <c r="H19" t="s">
-        <v>137</v>
+        <v>95</v>
+      </c>
+      <c r="G19" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
       </c>
       <c r="I19" t="str">
         <f t="array" ref="I19">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
@@ -2730,9 +2767,9 @@
         <f t="array" ref="J19">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
         <v/>
       </c>
-      <c r="K19" t="str">
+      <c r="K19" t="b">
         <f t="array" ref="K19">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="L19" t="str">
         <f t="array" ref="L19">IF( SUM((Courses[[#This Row],[Code]] = Spring_2018[Code]) * 1), TRUE(), "")</f>
@@ -2742,23 +2779,27 @@
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 6045</v>
+        <v>SYS 6005</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="9">
-        <v>6045</v>
+        <v>6005</v>
       </c>
       <c r="D20" t="s">
-        <v>75</v>
-      </c>
-      <c r="G20" t="s">
-        <v>155</v>
-      </c>
-      <c r="I20" t="str">
+        <v>59</v>
+      </c>
+      <c r="E20" t="s">
+        <v>95</v>
+      </c>
+      <c r="G20" t="b">
+        <f>TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I20" t="b">
         <f t="array" ref="I20">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="J20" t="str">
         <f t="array" ref="J20">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
@@ -2776,22 +2817,16 @@
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 6050</v>
+        <v>SYS 6013</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="9">
-        <v>6050</v>
+        <v>6013</v>
       </c>
       <c r="D21" t="s">
-        <v>76</v>
-      </c>
-      <c r="E21" t="s">
-        <v>103</v>
-      </c>
-      <c r="F21" t="s">
-        <v>130</v>
+        <v>63</v>
       </c>
       <c r="G21" t="s">
         <v>155</v>
@@ -2816,22 +2851,19 @@
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 6054</v>
+        <v>SYS 6014</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="9">
-        <v>6054</v>
+        <v>6014</v>
       </c>
       <c r="D22" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="E22" t="s">
-        <v>105</v>
-      </c>
-      <c r="F22" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="G22" t="s">
         <v>155</v>
@@ -2856,16 +2888,19 @@
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 6064</v>
+        <v>SYS 6026</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="9">
-        <v>6064</v>
+        <v>6026</v>
       </c>
       <c r="D23" t="s">
-        <v>78</v>
+        <v>69</v>
+      </c>
+      <c r="E23" t="s">
+        <v>102</v>
       </c>
       <c r="G23" t="s">
         <v>155</v>
@@ -2890,22 +2925,16 @@
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 6070</v>
+        <v>SYS 6042</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C24" s="9">
-        <v>6070</v>
+        <v>6042</v>
       </c>
       <c r="D24" t="s">
-        <v>79</v>
-      </c>
-      <c r="E24" t="s">
-        <v>106</v>
-      </c>
-      <c r="F24" t="s">
-        <v>131</v>
+        <v>72</v>
       </c>
       <c r="G24" t="s">
         <v>155</v>
@@ -2930,16 +2959,16 @@
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 6074</v>
+        <v>SYS 6043</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C25" s="9">
-        <v>6074</v>
+        <v>6043</v>
       </c>
       <c r="D25" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="G25" t="s">
         <v>155</v>
@@ -3084,25 +3113,19 @@
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 7001</v>
+        <v>SYS 6045</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C29" s="9">
-        <v>7001</v>
+        <v>6045</v>
       </c>
       <c r="D29" t="s">
-        <v>80</v>
-      </c>
-      <c r="E29" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
       <c r="G29" t="s">
         <v>155</v>
-      </c>
-      <c r="H29" t="s">
-        <v>137</v>
       </c>
       <c r="I29" t="str">
         <f t="array" ref="I29">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
@@ -3207,16 +3230,22 @@
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 7016</v>
+        <v>SYS 6050</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C32" s="9">
-        <v>7016</v>
+        <v>6050</v>
       </c>
       <c r="D32" t="s">
-        <v>83</v>
+        <v>76</v>
+      </c>
+      <c r="E32" t="s">
+        <v>103</v>
+      </c>
+      <c r="F32" t="s">
+        <v>130</v>
       </c>
       <c r="G32" t="s">
         <v>155</v>
@@ -3284,19 +3313,22 @@
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 7027</v>
+        <v>SYS 6054</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C34" s="9">
-        <v>7027</v>
+        <v>6054</v>
       </c>
       <c r="D34" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E34" t="s">
-        <v>111</v>
+        <v>105</v>
+      </c>
+      <c r="F34" t="s">
+        <v>130</v>
       </c>
       <c r="G34" t="s">
         <v>155</v>
@@ -3321,16 +3353,16 @@
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 7030</v>
+        <v>SYS 6064</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C35" s="9">
-        <v>7030</v>
+        <v>6064</v>
       </c>
       <c r="D35" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G35" t="s">
         <v>155</v>
@@ -3355,16 +3387,22 @@
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 7034</v>
+        <v>SYS 6070</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C36" s="9">
-        <v>7034</v>
+        <v>6070</v>
       </c>
       <c r="D36" t="s">
-        <v>87</v>
+        <v>79</v>
+      </c>
+      <c r="E36" t="s">
+        <v>106</v>
+      </c>
+      <c r="F36" t="s">
+        <v>131</v>
       </c>
       <c r="G36" t="s">
         <v>155</v>
@@ -3389,16 +3427,16 @@
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 7042</v>
+        <v>SYS 6074</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C37" s="9">
-        <v>7042</v>
+        <v>6074</v>
       </c>
       <c r="D37" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="G37" t="s">
         <v>155</v>
@@ -3466,19 +3504,16 @@
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 7052</v>
+        <v>SYS 7016</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C39" s="9">
-        <v>7052</v>
+        <v>7016</v>
       </c>
       <c r="D39" t="s">
-        <v>89</v>
-      </c>
-      <c r="E39" t="s">
-        <v>112</v>
+        <v>83</v>
       </c>
       <c r="G39" t="s">
         <v>155</v>
@@ -3503,16 +3538,19 @@
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 7054</v>
+        <v>SYS 7027</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C40" s="9">
-        <v>7054</v>
+        <v>7027</v>
       </c>
       <c r="D40" t="s">
-        <v>90</v>
+        <v>85</v>
+      </c>
+      <c r="E40" t="s">
+        <v>111</v>
       </c>
       <c r="G40" t="s">
         <v>155</v>
@@ -3577,16 +3615,16 @@
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 7070</v>
+        <v>SYS 7030</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C42" s="9">
-        <v>7070</v>
+        <v>7030</v>
       </c>
       <c r="D42" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="G42" t="s">
         <v>155</v>
@@ -3611,19 +3649,16 @@
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 7075</v>
+        <v>SYS 7034</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C43" s="9">
-        <v>7075</v>
+        <v>7034</v>
       </c>
       <c r="D43" t="s">
-        <v>93</v>
-      </c>
-      <c r="E43" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="G43" t="s">
         <v>155</v>
@@ -3645,505 +3680,480 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
+        <v>SYS 7042</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="9">
+        <v>7042</v>
+      </c>
+      <c r="D44" t="s">
+        <v>88</v>
+      </c>
+      <c r="G44" t="s">
+        <v>155</v>
+      </c>
+      <c r="I44" t="str">
+        <f t="array" ref="I44">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="J44" t="str">
+        <f t="array" ref="J44">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="K44" t="str">
+        <f t="array" ref="K44">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="L44" t="str">
+        <f t="array" ref="L44">IF( SUM((Courses[[#This Row],[Code]] = Spring_2018[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" t="str">
+        <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
+        <v>SYS 7097</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" s="9">
+        <v>7097</v>
+      </c>
+      <c r="D45" t="s">
+        <v>119</v>
+      </c>
+      <c r="E45" t="s">
+        <v>120</v>
+      </c>
+      <c r="G45" t="s">
+        <v>155</v>
+      </c>
+      <c r="H45" t="s">
+        <v>136</v>
+      </c>
+      <c r="I45" t="str">
+        <f t="array" ref="I45">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="J45" t="str">
+        <f t="array" ref="J45">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="K45" t="str">
+        <f t="array" ref="K45">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="L45" t="str">
+        <f t="array" ref="L45">IF( SUM((Courses[[#This Row],[Code]] = Spring_2018[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" t="str">
+        <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
+        <v>SYS 7581</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="9">
+        <v>7581</v>
+      </c>
+      <c r="D46" t="s">
+        <v>121</v>
+      </c>
+      <c r="E46" t="s">
+        <v>122</v>
+      </c>
+      <c r="G46" t="s">
+        <v>155</v>
+      </c>
+      <c r="H46" t="s">
+        <v>136</v>
+      </c>
+      <c r="I46" t="str">
+        <f t="array" ref="I46">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="J46" t="str">
+        <f t="array" ref="J46">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="K46" t="str">
+        <f t="array" ref="K46">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="L46" t="str">
+        <f t="array" ref="L46">IF( SUM((Courses[[#This Row],[Code]] = Spring_2018[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" t="str">
+        <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
+        <v>SYS 7582</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" s="9">
+        <v>7582</v>
+      </c>
+      <c r="D47" t="s">
+        <v>123</v>
+      </c>
+      <c r="E47" t="s">
+        <v>124</v>
+      </c>
+      <c r="G47" t="s">
+        <v>155</v>
+      </c>
+      <c r="H47" t="s">
+        <v>136</v>
+      </c>
+      <c r="I47" t="str">
+        <f t="array" ref="I47">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="J47" t="str">
+        <f t="array" ref="J47">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="K47" t="str">
+        <f t="array" ref="K47">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="L47" t="str">
+        <f t="array" ref="L47">IF( SUM((Courses[[#This Row],[Code]] = Spring_2018[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A48" t="str">
+        <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
+        <v>SYS 7993</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="9">
+        <v>7993</v>
+      </c>
+      <c r="D48" t="s">
+        <v>26</v>
+      </c>
+      <c r="E48" t="s">
+        <v>100</v>
+      </c>
+      <c r="G48" t="s">
+        <v>155</v>
+      </c>
+      <c r="H48" t="s">
+        <v>136</v>
+      </c>
+      <c r="I48" t="str">
+        <f t="array" ref="I48">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="J48" t="str">
+        <f t="array" ref="J48">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="K48" t="str">
+        <f t="array" ref="K48">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="L48" t="str">
+        <f t="array" ref="L48">IF( SUM((Courses[[#This Row],[Code]] = Spring_2018[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" t="str">
+        <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
+        <v>SYS 7052</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" s="9">
+        <v>7052</v>
+      </c>
+      <c r="D49" t="s">
+        <v>89</v>
+      </c>
+      <c r="E49" t="s">
+        <v>112</v>
+      </c>
+      <c r="G49" t="s">
+        <v>155</v>
+      </c>
+      <c r="I49" t="str">
+        <f t="array" ref="I49">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="J49" t="str">
+        <f t="array" ref="J49">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="K49" t="str">
+        <f t="array" ref="K49">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="L49" t="str">
+        <f t="array" ref="L49">IF( SUM((Courses[[#This Row],[Code]] = Spring_2018[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" t="str">
+        <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
+        <v>SYS 7054</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="9">
+        <v>7054</v>
+      </c>
+      <c r="D50" t="s">
+        <v>90</v>
+      </c>
+      <c r="G50" t="s">
+        <v>155</v>
+      </c>
+      <c r="I50" t="str">
+        <f t="array" ref="I50">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="J50" t="str">
+        <f t="array" ref="J50">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="K50" t="str">
+        <f t="array" ref="K50">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="L50" t="str">
+        <f t="array" ref="L50">IF( SUM((Courses[[#This Row],[Code]] = Spring_2018[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" t="str">
+        <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
+        <v>SYS 7070</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="9">
+        <v>7070</v>
+      </c>
+      <c r="D51" t="s">
+        <v>92</v>
+      </c>
+      <c r="G51" t="s">
+        <v>155</v>
+      </c>
+      <c r="I51" t="str">
+        <f t="array" ref="I51">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="J51" t="str">
+        <f t="array" ref="J51">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="K51" t="str">
+        <f t="array" ref="K51">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="L51" t="str">
+        <f t="array" ref="L51">IF( SUM((Courses[[#This Row],[Code]] = Spring_2018[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" t="str">
+        <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
+        <v>SYS 7075</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" s="9">
+        <v>7075</v>
+      </c>
+      <c r="D52" t="s">
+        <v>93</v>
+      </c>
+      <c r="E52" t="s">
+        <v>114</v>
+      </c>
+      <c r="G52" t="s">
+        <v>155</v>
+      </c>
+      <c r="I52" t="str">
+        <f t="array" ref="I52">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="J52" t="str">
+        <f t="array" ref="J52">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="K52" t="str">
+        <f t="array" ref="K52">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="L52" t="str">
+        <f t="array" ref="L52">IF( SUM((Courses[[#This Row],[Code]] = Spring_2018[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" t="str">
+        <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
         <v>SYS 7096</v>
       </c>
-      <c r="B44" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="9">
+      <c r="B53" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="9">
         <v>7096</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D53" t="s">
         <v>8</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E53" t="s">
         <v>100</v>
       </c>
-      <c r="G44" t="b">
+      <c r="G53" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I44" t="b">
-        <f t="array" ref="I44">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
+      <c r="I53" t="b">
+        <f t="array" ref="I53">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
         <v>1</v>
       </c>
-      <c r="J44" t="b">
-        <f t="array" ref="J44">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
+      <c r="J53" t="b">
+        <f t="array" ref="J53">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
         <v>1</v>
       </c>
-      <c r="K44" t="str">
-        <f t="array" ref="K44">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="L44" t="str">
-        <f t="array" ref="L44">IF( SUM((Courses[[#This Row],[Code]] = Spring_2018[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A45" t="str">
-        <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 7097</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C45" s="9">
-        <v>7097</v>
-      </c>
-      <c r="D45" t="s">
-        <v>119</v>
-      </c>
-      <c r="E45" t="s">
-        <v>120</v>
-      </c>
-      <c r="G45" t="s">
-        <v>155</v>
-      </c>
-      <c r="H45" t="s">
-        <v>136</v>
-      </c>
-      <c r="I45" t="str">
-        <f t="array" ref="I45">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="J45" t="str">
-        <f t="array" ref="J45">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="K45" t="str">
-        <f t="array" ref="K45">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="L45" t="str">
-        <f t="array" ref="L45">IF( SUM((Courses[[#This Row],[Code]] = Spring_2018[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A46" t="str">
-        <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 7581</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C46" s="9">
-        <v>7581</v>
-      </c>
-      <c r="D46" t="s">
-        <v>121</v>
-      </c>
-      <c r="E46" t="s">
-        <v>122</v>
-      </c>
-      <c r="G46" t="s">
-        <v>155</v>
-      </c>
-      <c r="H46" t="s">
-        <v>136</v>
-      </c>
-      <c r="I46" t="str">
-        <f t="array" ref="I46">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="J46" t="str">
-        <f t="array" ref="J46">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="K46" t="str">
-        <f t="array" ref="K46">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="L46" t="str">
-        <f t="array" ref="L46">IF( SUM((Courses[[#This Row],[Code]] = Spring_2018[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A47" t="str">
-        <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 7582</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C47" s="9">
-        <v>7582</v>
-      </c>
-      <c r="D47" t="s">
-        <v>123</v>
-      </c>
-      <c r="E47" t="s">
-        <v>124</v>
-      </c>
-      <c r="G47" t="s">
-        <v>155</v>
-      </c>
-      <c r="H47" t="s">
-        <v>136</v>
-      </c>
-      <c r="I47" t="str">
-        <f t="array" ref="I47">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="J47" t="str">
-        <f t="array" ref="J47">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="K47" t="str">
-        <f t="array" ref="K47">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="L47" t="str">
-        <f t="array" ref="L47">IF( SUM((Courses[[#This Row],[Code]] = Spring_2018[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A48" t="str">
-        <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 7993</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C48" s="9">
-        <v>7993</v>
-      </c>
-      <c r="D48" t="s">
-        <v>26</v>
-      </c>
-      <c r="E48" t="s">
+      <c r="K53" t="str">
+        <f t="array" ref="K53">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="L53" t="str">
+        <f t="array" ref="L53">IF( SUM((Courses[[#This Row],[Code]] = Spring_2018[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" t="str">
+        <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
+        <v>SYS 8995</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" s="9">
+        <v>8995</v>
+      </c>
+      <c r="D54" t="s">
+        <v>115</v>
+      </c>
+      <c r="E54" t="s">
         <v>100</v>
       </c>
-      <c r="G48" t="s">
-        <v>155</v>
-      </c>
-      <c r="H48" t="s">
-        <v>136</v>
-      </c>
-      <c r="I48" t="str">
-        <f t="array" ref="I48">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="J48" t="str">
-        <f t="array" ref="J48">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="K48" t="str">
-        <f t="array" ref="K48">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="L48" t="str">
-        <f t="array" ref="L48">IF( SUM((Courses[[#This Row],[Code]] = Spring_2018[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A49" t="str">
-        <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SYS 8995</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C49" s="9">
-        <v>8995</v>
-      </c>
-      <c r="D49" t="s">
-        <v>115</v>
-      </c>
-      <c r="E49" t="s">
-        <v>100</v>
-      </c>
-      <c r="G49" t="b">
+      <c r="G54" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I49" t="str">
-        <f t="array" ref="I49">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="J49" t="str">
-        <f t="array" ref="J49">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="K49" t="b">
-        <f t="array" ref="K49">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
+      <c r="I54" t="str">
+        <f t="array" ref="I54">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="J54" t="str">
+        <f t="array" ref="J54">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="K54" t="b">
+        <f t="array" ref="K54">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
         <v>1</v>
       </c>
-      <c r="L49" t="b">
-        <f t="array" ref="L49">IF( SUM((Courses[[#This Row],[Code]] = Spring_2018[Code]) * 1), TRUE(), "")</f>
+      <c r="L54" t="b">
+        <f t="array" ref="L54">IF( SUM((Courses[[#This Row],[Code]] = Spring_2018[Code]) * 1), TRUE(), "")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A50" t="str">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
         <v>SYS 8997</v>
       </c>
-      <c r="B50" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C50" s="9">
+      <c r="B55" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" s="9">
         <v>8997</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D55" t="s">
         <v>116</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E55" t="s">
         <v>100</v>
       </c>
-      <c r="F50" s="6" t="s">
+      <c r="F55" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="G50" t="b">
+      <c r="G55" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I50" t="b">
-        <f t="array" ref="I50">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
+      <c r="I55" t="b">
+        <f t="array" ref="I55">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
         <v>1</v>
       </c>
-      <c r="J50" t="b">
-        <f t="array" ref="J50">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
+      <c r="J55" t="b">
+        <f t="array" ref="J55">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
         <v>1</v>
       </c>
-      <c r="K50" t="str">
-        <f t="array" ref="K50">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="L50" t="str">
-        <f t="array" ref="L50">IF( SUM((Courses[[#This Row],[Code]] = Spring_2018[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A51" t="str">
+      <c r="K55" t="str">
+        <f t="array" ref="K55">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+      <c r="L55" t="str">
+        <f t="array" ref="L55">IF( SUM((Courses[[#This Row],[Code]] = Spring_2018[Code]) * 1), TRUE(), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
         <v>SYS 8999</v>
       </c>
-      <c r="B51" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C51" s="9">
+      <c r="B56" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="9">
         <v>8999</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D56" t="s">
         <v>11</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E56" t="s">
         <v>100</v>
       </c>
-      <c r="G51" t="b">
+      <c r="G56" t="b">
         <f>TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I51" t="str">
-        <f t="array" ref="I51">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="J51" t="str">
-        <f t="array" ref="J51">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="K51" t="b">
-        <f t="array" ref="K51">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
-        <v>1</v>
-      </c>
-      <c r="L51" t="b">
-        <f t="array" ref="L51">IF( SUM((Courses[[#This Row],[Code]] = Spring_2018[Code]) * 1), TRUE(), "")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" t="str">
-        <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>SOC 5120</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="C52" s="9">
-        <v>5120</v>
-      </c>
-      <c r="D52" t="s">
-        <v>152</v>
-      </c>
-      <c r="E52" t="s">
-        <v>103</v>
-      </c>
-      <c r="G52" t="s">
-        <v>155</v>
-      </c>
-      <c r="H52" t="s">
-        <v>137</v>
-      </c>
-      <c r="I52" t="str">
-        <f t="array" ref="I52">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="J52" t="str">
-        <f t="array" ref="J52">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="K52" t="str">
-        <f t="array" ref="K52">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="L52" t="str">
-        <f t="array" ref="L52">IF( SUM((Courses[[#This Row],[Code]] = Spring_2018[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" t="str">
-        <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>PSYC 7700</v>
-      </c>
-      <c r="B53" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="C53" s="9">
-        <v>7700</v>
-      </c>
-      <c r="D53" t="s">
-        <v>160</v>
-      </c>
-      <c r="E53" t="s">
-        <v>161</v>
-      </c>
-      <c r="G53" t="s">
-        <v>155</v>
-      </c>
-      <c r="H53" t="s">
-        <v>137</v>
-      </c>
-      <c r="I53" t="str">
-        <f t="array" ref="I53">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="J53" t="str">
-        <f t="array" ref="J53">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="K53" t="str">
-        <f t="array" ref="K53">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="L53" t="str">
-        <f t="array" ref="L53">IF( SUM((Courses[[#This Row],[Code]] = Spring_2018[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" t="str">
-        <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>PSYC 7710</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="C54" s="9">
-        <v>7710</v>
-      </c>
-      <c r="D54" t="s">
-        <v>162</v>
-      </c>
-      <c r="E54" t="s">
-        <v>95</v>
-      </c>
-      <c r="G54" t="s">
-        <v>155</v>
-      </c>
-      <c r="I54" t="str">
-        <f t="array" ref="I54">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="J54" t="str">
-        <f t="array" ref="J54">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="K54" t="str">
-        <f t="array" ref="K54">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="L54" t="str">
-        <f t="array" ref="L54">IF( SUM((Courses[[#This Row],[Code]] = Spring_2018[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A55" s="8" t="str">
-        <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>PSYC 8730</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="C55" s="9">
-        <v>8730</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="E55" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="F55" s="7"/>
-      <c r="G55" t="s">
-        <v>155</v>
-      </c>
-      <c r="H55" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="I55" s="7" t="str">
-        <f t="array" ref="I55">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="J55" s="7" t="str">
-        <f t="array" ref="J55">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="K55" s="7" t="str">
-        <f t="array" ref="K55">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="L55" s="8" t="str">
-        <f t="array" ref="L55">IF( SUM((Courses[[#This Row],[Code]] = Spring_2018[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A56" t="str">
-        <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>PLAN 5630</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="C56" s="9">
-        <v>5630</v>
-      </c>
-      <c r="D56" t="s">
-        <v>150</v>
-      </c>
-      <c r="E56" t="s">
-        <v>159</v>
-      </c>
-      <c r="F56" t="s">
-        <v>151</v>
-      </c>
-      <c r="G56" t="s">
-        <v>155</v>
-      </c>
-      <c r="H56" t="s">
-        <v>137</v>
-      </c>
       <c r="I56" t="str">
         <f t="array" ref="I56">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
         <v/>
@@ -4152,37 +4162,34 @@
         <f t="array" ref="J56">IF( SUM((Courses[[#This Row],[Code]] = Spring_2017[Code]) * 1), TRUE(), "")</f>
         <v/>
       </c>
-      <c r="K56" t="str">
+      <c r="K56" t="b">
         <f t="array" ref="K56">IF( SUM((Courses[[#This Row],[Code]] = Fall_2017[Code]) * 1), TRUE(), "")</f>
-        <v/>
-      </c>
-      <c r="L56" t="str">
+        <v>1</v>
+      </c>
+      <c r="L56" t="b">
         <f t="array" ref="L56">IF( SUM((Courses[[#This Row],[Code]] = Spring_2018[Code]) * 1), TRUE(), "")</f>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
         <f>Courses[[#This Row],[Dpmt]] &amp; " " &amp; Courses[[#This Row],[Num]]</f>
-        <v>PPOL 5025</v>
+        <v>PSYC 7710</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="C57" s="9">
-        <v>5025</v>
+        <v>7710</v>
       </c>
       <c r="D57" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="E57" t="s">
-        <v>158</v>
+        <v>95</v>
       </c>
       <c r="G57" t="s">
         <v>155</v>
-      </c>
-      <c r="H57" t="s">
-        <v>137</v>
       </c>
       <c r="I57" t="str">
         <f t="array" ref="I57">IF( SUM((Courses[[#This Row],[Code]] = Fall_2016[Code]) * 1), TRUE(), "")</f>
@@ -4242,7 +4249,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F50" r:id="rId1"/>
+    <hyperlink ref="F55" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>